<commit_message>
15.01.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/15.01.2020 Requisition of Mughdo Corporation.xlsx
+++ b/2020/Requisition/15.01.2020 Requisition of Mughdo Corporation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\Requisition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E566797-C433-42AB-B3BC-2E9C0DCCEDA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DA2B36-BE15-42AE-966A-D990C8F0D84C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="133">
   <si>
     <t>Model Name</t>
   </si>
@@ -438,7 +438,10 @@
     <t>15.01.2020</t>
   </si>
   <si>
-    <t>Gold=100 Darkblue=60 Black=46</t>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Gold Only</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1102,10 @@
   <dimension ref="A1:BV108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
+      <selection pane="bottomRight" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1995,14 +1998,14 @@
         <v>1014.53</v>
       </c>
       <c r="C26" s="8">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>208993.18</v>
+        <v>283053.87</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -2435,19 +2438,17 @@
       <c r="BU36" s="26"/>
       <c r="BV36" s="26"/>
     </row>
-    <row r="37" spans="1:74" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>107</v>
       </c>
       <c r="B37" s="9">
         <v>5412.5</v>
       </c>
-      <c r="C37" s="8">
-        <v>40</v>
-      </c>
+      <c r="C37" s="8"/>
       <c r="D37" s="10">
         <f>C37*B37</f>
-        <v>216500</v>
+        <v>0</v>
       </c>
       <c r="E37" s="41" t="s">
         <v>125</v>
@@ -3740,19 +3741,17 @@
       <c r="BB90" s="32"/>
       <c r="BC90" s="32"/>
     </row>
-    <row r="91" spans="1:74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:74" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>103</v>
       </c>
       <c r="B91" s="9">
         <v>1072.675</v>
       </c>
-      <c r="C91" s="8">
-        <v>60</v>
-      </c>
+      <c r="C91" s="8"/>
       <c r="D91" s="10">
         <f t="shared" si="2"/>
-        <v>64360.5</v>
+        <v>0</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>92</v>
@@ -3816,14 +3815,14 @@
         <v>7165.02</v>
       </c>
       <c r="C92" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D92" s="10">
         <f t="shared" si="2"/>
-        <v>93145.260000000009</v>
+        <v>107475.3</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="F92" s="32"/>
       <c r="G92" s="32"/>
@@ -3891,7 +3890,7 @@
         <v>69221.430000000008</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -3931,11 +3930,11 @@
       <c r="B96" s="45"/>
       <c r="C96" s="16">
         <f>SUBTOTAL(9,C7:C95)</f>
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="D96" s="17">
         <f>SUBTOTAL(9,D7:D95)</f>
-        <v>652220.37</v>
+        <v>459750.6</v>
       </c>
       <c r="E96" s="31"/>
       <c r="F96" s="33"/>

</xml_diff>